<commit_message>
ADD seccion 4 completa
</commit_message>
<xml_diff>
--- a/inputs/Notas_Alumnos.xlsx
+++ b/inputs/Notas_Alumnos.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEC1232-B513-4DCC-BA98-C08A9B031241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6887A579-1413-43C8-BBB1-A9F25B55DCF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -241,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -262,11 +262,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A324" zoomScale="87" workbookViewId="0">
-      <selection activeCell="A357" sqref="A357:XFD357"/>
+    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166:XFD166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6612,20 +6607,20 @@
         <v>8.9922269914382067</v>
       </c>
     </row>
-    <row r="357" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A357" s="8" t="s">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A357" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B357" s="8" t="s">
+      <c r="B357" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C357" s="9">
+      <c r="C357" s="3">
         <v>3.2741364222589313</v>
       </c>
-      <c r="D357" s="9">
+      <c r="D357" s="3">
         <v>1.9839087899529706</v>
       </c>
-      <c r="E357" s="9">
+      <c r="E357" s="3">
         <v>1.6032283154539524</v>
       </c>
     </row>

</xml_diff>